<commit_message>
CIERRE  27 ABR 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #04  ABRIL   2022/ENTRADAS OBRADOR  ABRIL    2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #04  ABRIL   2022/ENTRADAS OBRADOR  ABRIL    2022.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="391">
   <si>
     <t>FECHA DE PAGO</t>
   </si>
@@ -1144,6 +1144,63 @@
   </si>
   <si>
     <t>0594 Z</t>
+  </si>
+  <si>
+    <t>0606 Z</t>
+  </si>
+  <si>
+    <t>0615 Z</t>
+  </si>
+  <si>
+    <t>0630 Z</t>
+  </si>
+  <si>
+    <t>0640 Z</t>
+  </si>
+  <si>
+    <t>0658 Z</t>
+  </si>
+  <si>
+    <t>0670 Z</t>
+  </si>
+  <si>
+    <t>0681 Z</t>
+  </si>
+  <si>
+    <t>20333--</t>
+  </si>
+  <si>
+    <t>20351--</t>
+  </si>
+  <si>
+    <t>20365--</t>
+  </si>
+  <si>
+    <t>20372--</t>
+  </si>
+  <si>
+    <t>20322--</t>
+  </si>
+  <si>
+    <t>20324--</t>
+  </si>
+  <si>
+    <t>20307--10837</t>
+  </si>
+  <si>
+    <t>20307--10835</t>
+  </si>
+  <si>
+    <t>20312--8770</t>
+  </si>
+  <si>
+    <t>20312--4738--NC-188</t>
+  </si>
+  <si>
+    <t>CHULETA MARIPOSA</t>
+  </si>
+  <si>
+    <t>FOLIO 10788</t>
   </si>
 </sst>
 </file>
@@ -3766,6 +3823,78 @@
     <xf numFmtId="164" fontId="22" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3799,84 +3928,12 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="22" fillId="11" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3907,6 +3964,12 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="32" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="32" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3938,12 +4001,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="18" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="32" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="32" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4274,18 +4331,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="480" t="s">
+      <c r="A1" s="504" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="480"/>
-      <c r="C1" s="480"/>
-      <c r="D1" s="480"/>
-      <c r="E1" s="480"/>
-      <c r="F1" s="480"/>
-      <c r="G1" s="480"/>
-      <c r="H1" s="480"/>
-      <c r="I1" s="480"/>
-      <c r="J1" s="480"/>
+      <c r="B1" s="504"/>
+      <c r="C1" s="504"/>
+      <c r="D1" s="504"/>
+      <c r="E1" s="504"/>
+      <c r="F1" s="504"/>
+      <c r="G1" s="504"/>
+      <c r="H1" s="504"/>
+      <c r="I1" s="504"/>
+      <c r="J1" s="504"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -4299,22 +4356,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="481" t="s">
+      <c r="W1" s="505" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="482"/>
+      <c r="X1" s="506"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="480"/>
-      <c r="B2" s="480"/>
-      <c r="C2" s="480"/>
-      <c r="D2" s="480"/>
-      <c r="E2" s="480"/>
-      <c r="F2" s="480"/>
-      <c r="G2" s="480"/>
-      <c r="H2" s="480"/>
-      <c r="I2" s="480"/>
-      <c r="J2" s="480"/>
+      <c r="A2" s="504"/>
+      <c r="B2" s="504"/>
+      <c r="C2" s="504"/>
+      <c r="D2" s="504"/>
+      <c r="E2" s="504"/>
+      <c r="F2" s="504"/>
+      <c r="G2" s="504"/>
+      <c r="H2" s="504"/>
+      <c r="I2" s="504"/>
+      <c r="J2" s="504"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -4368,10 +4425,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="483" t="s">
+      <c r="O3" s="507" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="484"/>
+      <c r="P3" s="508"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -4915,7 +4972,7 @@
       <c r="B12" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="485" t="s">
+      <c r="C12" s="509" t="s">
         <v>103</v>
       </c>
       <c r="D12" s="400"/>
@@ -4979,7 +5036,7 @@
       <c r="B13" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="486"/>
+      <c r="C13" s="510"/>
       <c r="D13" s="400"/>
       <c r="E13" s="401"/>
       <c r="F13" s="402">
@@ -6981,13 +7038,13 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="497" t="s">
+      <c r="A56" s="488" t="s">
         <v>41</v>
       </c>
       <c r="B56" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C56" s="499" t="s">
+      <c r="C56" s="490" t="s">
         <v>110</v>
       </c>
       <c r="D56" s="150"/>
@@ -6998,7 +7055,7 @@
       <c r="G56" s="152">
         <v>44571</v>
       </c>
-      <c r="H56" s="491">
+      <c r="H56" s="492">
         <v>782</v>
       </c>
       <c r="I56" s="151">
@@ -7027,11 +7084,11 @@
       <c r="V56" s="160"/>
     </row>
     <row r="57" spans="1:24" s="161" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="498"/>
+      <c r="A57" s="489"/>
       <c r="B57" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="500"/>
+      <c r="C57" s="491"/>
       <c r="D57" s="150"/>
       <c r="E57" s="40"/>
       <c r="F57" s="151">
@@ -7040,7 +7097,7 @@
       <c r="G57" s="152">
         <v>44571</v>
       </c>
-      <c r="H57" s="492"/>
+      <c r="H57" s="493"/>
       <c r="I57" s="151">
         <v>319</v>
       </c>
@@ -7067,13 +7124,13 @@
       <c r="V57" s="160"/>
     </row>
     <row r="58" spans="1:24" s="161" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="497" t="s">
+      <c r="A58" s="488" t="s">
         <v>41</v>
       </c>
       <c r="B58" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="499" t="s">
+      <c r="C58" s="490" t="s">
         <v>129</v>
       </c>
       <c r="D58" s="150"/>
@@ -7084,7 +7141,7 @@
       <c r="G58" s="152">
         <v>44578</v>
       </c>
-      <c r="H58" s="491">
+      <c r="H58" s="492">
         <v>810</v>
       </c>
       <c r="I58" s="151">
@@ -7103,10 +7160,10 @@
         <f t="shared" si="1"/>
         <v>75875.8</v>
       </c>
-      <c r="O58" s="493" t="s">
+      <c r="O58" s="494" t="s">
         <v>59</v>
       </c>
-      <c r="P58" s="495">
+      <c r="P58" s="515">
         <v>44606</v>
       </c>
       <c r="Q58" s="128"/>
@@ -7117,11 +7174,11 @@
       <c r="V58" s="160"/>
     </row>
     <row r="59" spans="1:24" s="161" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="498"/>
+      <c r="A59" s="489"/>
       <c r="B59" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C59" s="500"/>
+      <c r="C59" s="491"/>
       <c r="D59" s="150"/>
       <c r="E59" s="40"/>
       <c r="F59" s="151">
@@ -7130,7 +7187,7 @@
       <c r="G59" s="152">
         <v>44578</v>
       </c>
-      <c r="H59" s="492"/>
+      <c r="H59" s="493"/>
       <c r="I59" s="151">
         <v>220</v>
       </c>
@@ -7147,8 +7204,8 @@
         <f t="shared" si="1"/>
         <v>22440</v>
       </c>
-      <c r="O59" s="494"/>
-      <c r="P59" s="496"/>
+      <c r="O59" s="495"/>
+      <c r="P59" s="516"/>
       <c r="Q59" s="128"/>
       <c r="R59" s="158"/>
       <c r="S59" s="92"/>
@@ -7157,13 +7214,13 @@
       <c r="V59" s="160"/>
     </row>
     <row r="60" spans="1:24" s="161" customFormat="1" ht="48.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="489" t="s">
+      <c r="A60" s="513" t="s">
         <v>41</v>
       </c>
       <c r="B60" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C60" s="487" t="s">
+      <c r="C60" s="511" t="s">
         <v>109</v>
       </c>
       <c r="D60" s="163"/>
@@ -7177,7 +7234,7 @@
       <c r="G60" s="152">
         <v>44585</v>
       </c>
-      <c r="H60" s="491">
+      <c r="H60" s="492">
         <v>800</v>
       </c>
       <c r="I60" s="151">
@@ -7196,10 +7253,10 @@
         <f t="shared" si="1"/>
         <v>151187.4</v>
       </c>
-      <c r="O60" s="493" t="s">
+      <c r="O60" s="494" t="s">
         <v>59</v>
       </c>
-      <c r="P60" s="495">
+      <c r="P60" s="515">
         <v>44594</v>
       </c>
       <c r="Q60" s="164"/>
@@ -7212,11 +7269,11 @@
       <c r="X60"/>
     </row>
     <row r="61" spans="1:24" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="490"/>
+      <c r="A61" s="514"/>
       <c r="B61" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C61" s="488"/>
+      <c r="C61" s="512"/>
       <c r="D61" s="165"/>
       <c r="E61" s="40">
         <f t="shared" si="2"/>
@@ -7228,7 +7285,7 @@
       <c r="G61" s="152">
         <v>44585</v>
       </c>
-      <c r="H61" s="492"/>
+      <c r="H61" s="493"/>
       <c r="I61" s="151">
         <v>231.6</v>
       </c>
@@ -7245,8 +7302,8 @@
         <f t="shared" si="1"/>
         <v>23623.200000000001</v>
       </c>
-      <c r="O61" s="494"/>
-      <c r="P61" s="496"/>
+      <c r="O61" s="495"/>
+      <c r="P61" s="516"/>
       <c r="Q61" s="164"/>
       <c r="R61" s="129"/>
       <c r="S61" s="92"/>
@@ -7312,7 +7369,7 @@
       <c r="B63" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C63" s="513"/>
+      <c r="C63" s="482"/>
       <c r="D63" s="163"/>
       <c r="E63" s="40">
         <f t="shared" si="2"/>
@@ -7320,7 +7377,7 @@
       </c>
       <c r="F63" s="151"/>
       <c r="G63" s="152"/>
-      <c r="H63" s="515"/>
+      <c r="H63" s="484"/>
       <c r="I63" s="151"/>
       <c r="J63" s="45">
         <f t="shared" si="0"/>
@@ -7349,7 +7406,7 @@
       <c r="B64" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C64" s="514"/>
+      <c r="C64" s="483"/>
       <c r="D64" s="168"/>
       <c r="E64" s="40">
         <f t="shared" si="2"/>
@@ -7357,7 +7414,7 @@
       </c>
       <c r="F64" s="151"/>
       <c r="G64" s="152"/>
-      <c r="H64" s="516"/>
+      <c r="H64" s="485"/>
       <c r="I64" s="151"/>
       <c r="J64" s="45">
         <f t="shared" si="0"/>
@@ -7535,8 +7592,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O68" s="505"/>
-      <c r="P68" s="511"/>
+      <c r="O68" s="486"/>
+      <c r="P68" s="480"/>
       <c r="Q68" s="164"/>
       <c r="R68" s="129"/>
       <c r="S68" s="180"/>
@@ -7570,8 +7627,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O69" s="506"/>
-      <c r="P69" s="512"/>
+      <c r="O69" s="487"/>
+      <c r="P69" s="481"/>
       <c r="Q69" s="164"/>
       <c r="R69" s="129"/>
       <c r="S69" s="180"/>
@@ -8061,8 +8118,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="505"/>
-      <c r="P82" s="507"/>
+      <c r="O82" s="486"/>
+      <c r="P82" s="500"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="129"/>
       <c r="S82" s="180"/>
@@ -8094,8 +8151,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O83" s="506"/>
-      <c r="P83" s="508"/>
+      <c r="O83" s="487"/>
+      <c r="P83" s="501"/>
       <c r="Q83" s="164"/>
       <c r="R83" s="129"/>
       <c r="S83" s="180"/>
@@ -8127,8 +8184,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O84" s="505"/>
-      <c r="P84" s="507"/>
+      <c r="O84" s="486"/>
+      <c r="P84" s="500"/>
       <c r="Q84" s="164"/>
       <c r="R84" s="158"/>
       <c r="S84" s="180"/>
@@ -8160,8 +8217,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O85" s="506"/>
-      <c r="P85" s="508"/>
+      <c r="O85" s="487"/>
+      <c r="P85" s="501"/>
       <c r="Q85" s="164"/>
       <c r="R85" s="158"/>
       <c r="S85" s="180"/>
@@ -8319,8 +8376,8 @@
         <v>0</v>
       </c>
       <c r="K90" s="100"/>
-      <c r="L90" s="509"/>
-      <c r="M90" s="510"/>
+      <c r="L90" s="502"/>
+      <c r="M90" s="503"/>
       <c r="N90" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8352,8 +8409,8 @@
         <v>0</v>
       </c>
       <c r="K91" s="100"/>
-      <c r="L91" s="509"/>
-      <c r="M91" s="510"/>
+      <c r="L91" s="502"/>
+      <c r="M91" s="503"/>
       <c r="N91" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8556,8 +8613,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O97" s="505"/>
-      <c r="P97" s="501"/>
+      <c r="O97" s="486"/>
+      <c r="P97" s="496"/>
       <c r="Q97" s="164"/>
       <c r="R97" s="129"/>
       <c r="S97" s="180"/>
@@ -8589,8 +8646,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O98" s="506"/>
-      <c r="P98" s="502"/>
+      <c r="O98" s="487"/>
+      <c r="P98" s="497"/>
       <c r="Q98" s="164"/>
       <c r="R98" s="129"/>
       <c r="S98" s="180"/>
@@ -13982,11 +14039,11 @@
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F262" s="503" t="s">
+      <c r="F262" s="498" t="s">
         <v>26</v>
       </c>
-      <c r="G262" s="503"/>
-      <c r="H262" s="504"/>
+      <c r="G262" s="498"/>
+      <c r="H262" s="499"/>
       <c r="I262" s="317">
         <f>SUM(I4:I261)</f>
         <v>426245.47000000003</v>
@@ -14560,22 +14617,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="P68:P69"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="O68:O69"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="H58:H59"/>
-    <mergeCell ref="O58:O59"/>
-    <mergeCell ref="P97:P98"/>
-    <mergeCell ref="F262:H262"/>
-    <mergeCell ref="O82:O83"/>
-    <mergeCell ref="P82:P83"/>
-    <mergeCell ref="O84:O85"/>
-    <mergeCell ref="P84:P85"/>
-    <mergeCell ref="L90:M91"/>
-    <mergeCell ref="O97:O98"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="O3:P3"/>
@@ -14589,6 +14630,22 @@
     <mergeCell ref="C56:C57"/>
     <mergeCell ref="H56:H57"/>
     <mergeCell ref="P58:P59"/>
+    <mergeCell ref="P97:P98"/>
+    <mergeCell ref="F262:H262"/>
+    <mergeCell ref="O82:O83"/>
+    <mergeCell ref="P82:P83"/>
+    <mergeCell ref="O84:O85"/>
+    <mergeCell ref="P84:P85"/>
+    <mergeCell ref="L90:M91"/>
+    <mergeCell ref="O97:O98"/>
+    <mergeCell ref="P68:P69"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="H63:H64"/>
+    <mergeCell ref="O68:O69"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="O58:O59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -14632,18 +14689,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="480" t="s">
+      <c r="A1" s="504" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="480"/>
-      <c r="C1" s="480"/>
-      <c r="D1" s="480"/>
-      <c r="E1" s="480"/>
-      <c r="F1" s="480"/>
-      <c r="G1" s="480"/>
-      <c r="H1" s="480"/>
-      <c r="I1" s="480"/>
-      <c r="J1" s="480"/>
+      <c r="B1" s="504"/>
+      <c r="C1" s="504"/>
+      <c r="D1" s="504"/>
+      <c r="E1" s="504"/>
+      <c r="F1" s="504"/>
+      <c r="G1" s="504"/>
+      <c r="H1" s="504"/>
+      <c r="I1" s="504"/>
+      <c r="J1" s="504"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -14659,22 +14716,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="481" t="s">
+      <c r="W1" s="505" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="482"/>
+      <c r="X1" s="506"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="480"/>
-      <c r="B2" s="480"/>
-      <c r="C2" s="480"/>
-      <c r="D2" s="480"/>
-      <c r="E2" s="480"/>
-      <c r="F2" s="480"/>
-      <c r="G2" s="480"/>
-      <c r="H2" s="480"/>
-      <c r="I2" s="480"/>
-      <c r="J2" s="480"/>
+      <c r="A2" s="504"/>
+      <c r="B2" s="504"/>
+      <c r="C2" s="504"/>
+      <c r="D2" s="504"/>
+      <c r="E2" s="504"/>
+      <c r="F2" s="504"/>
+      <c r="G2" s="504"/>
+      <c r="H2" s="504"/>
+      <c r="I2" s="504"/>
+      <c r="J2" s="504"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -14728,10 +14785,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="483" t="s">
+      <c r="O3" s="507" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="484"/>
+      <c r="P3" s="508"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -17373,7 +17430,7 @@
       <c r="B55" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C55" s="499" t="s">
+      <c r="C55" s="490" t="s">
         <v>160</v>
       </c>
       <c r="D55" s="150"/>
@@ -17384,7 +17441,7 @@
       <c r="G55" s="152">
         <v>44599</v>
       </c>
-      <c r="H55" s="515" t="s">
+      <c r="H55" s="484" t="s">
         <v>161</v>
       </c>
       <c r="I55" s="151">
@@ -17417,7 +17474,7 @@
       <c r="B56" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="500"/>
+      <c r="C56" s="491"/>
       <c r="D56" s="163"/>
       <c r="E56" s="40"/>
       <c r="F56" s="151">
@@ -17426,7 +17483,7 @@
       <c r="G56" s="152">
         <v>44599</v>
       </c>
-      <c r="H56" s="516"/>
+      <c r="H56" s="485"/>
       <c r="I56" s="151">
         <v>194.4</v>
       </c>
@@ -17472,7 +17529,7 @@
       <c r="G57" s="152">
         <v>44606</v>
       </c>
-      <c r="H57" s="515" t="s">
+      <c r="H57" s="484" t="s">
         <v>163</v>
       </c>
       <c r="I57" s="151">
@@ -17491,10 +17548,10 @@
         <f t="shared" si="1"/>
         <v>35776</v>
       </c>
-      <c r="O57" s="505" t="s">
+      <c r="O57" s="486" t="s">
         <v>59</v>
       </c>
-      <c r="P57" s="511">
+      <c r="P57" s="480">
         <v>44620</v>
       </c>
       <c r="Q57" s="164"/>
@@ -17518,7 +17575,7 @@
       <c r="G58" s="152">
         <v>44606</v>
       </c>
-      <c r="H58" s="516"/>
+      <c r="H58" s="485"/>
       <c r="I58" s="151">
         <v>627.60209999999995</v>
       </c>
@@ -17562,7 +17619,7 @@
       <c r="G59" s="152">
         <v>44613</v>
       </c>
-      <c r="H59" s="515" t="s">
+      <c r="H59" s="484" t="s">
         <v>225</v>
       </c>
       <c r="I59" s="151">
@@ -17606,7 +17663,7 @@
       <c r="E60" s="40"/>
       <c r="F60" s="151"/>
       <c r="G60" s="152"/>
-      <c r="H60" s="516"/>
+      <c r="H60" s="485"/>
       <c r="I60" s="151"/>
       <c r="J60" s="45">
         <f t="shared" si="0"/>
@@ -18269,8 +18326,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="505"/>
-      <c r="P79" s="507"/>
+      <c r="O79" s="486"/>
+      <c r="P79" s="500"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -18299,8 +18356,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="506"/>
-      <c r="P80" s="508"/>
+      <c r="O80" s="487"/>
+      <c r="P80" s="501"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -18329,8 +18386,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="505"/>
-      <c r="P81" s="507"/>
+      <c r="O81" s="486"/>
+      <c r="P81" s="500"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -18362,8 +18419,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="506"/>
-      <c r="P82" s="508"/>
+      <c r="O82" s="487"/>
+      <c r="P82" s="501"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -18521,8 +18578,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="509"/>
-      <c r="M87" s="510"/>
+      <c r="L87" s="502"/>
+      <c r="M87" s="503"/>
       <c r="N87" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -18554,8 +18611,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="509"/>
-      <c r="M88" s="510"/>
+      <c r="L88" s="502"/>
+      <c r="M88" s="503"/>
       <c r="N88" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -18758,8 +18815,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="505"/>
-      <c r="P94" s="501"/>
+      <c r="O94" s="486"/>
+      <c r="P94" s="496"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -18791,8 +18848,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="506"/>
-      <c r="P95" s="502"/>
+      <c r="O95" s="487"/>
+      <c r="P95" s="497"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -24184,11 +24241,11 @@
         <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="503" t="s">
+      <c r="F259" s="498" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="503"/>
-      <c r="H259" s="504"/>
+      <c r="G259" s="498"/>
+      <c r="H259" s="499"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>387207.97210000001</v>
@@ -24762,6 +24819,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="L87:M88"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
     <mergeCell ref="O79:O80"/>
     <mergeCell ref="P79:P80"/>
     <mergeCell ref="A1:J2"/>
@@ -24777,12 +24840,6 @@
     <mergeCell ref="C55:C56"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="H55:H56"/>
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="L87:M88"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -24829,18 +24886,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="480" t="s">
+      <c r="A1" s="504" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="480"/>
-      <c r="C1" s="480"/>
-      <c r="D1" s="480"/>
-      <c r="E1" s="480"/>
-      <c r="F1" s="480"/>
-      <c r="G1" s="480"/>
-      <c r="H1" s="480"/>
-      <c r="I1" s="480"/>
-      <c r="J1" s="480"/>
+      <c r="B1" s="504"/>
+      <c r="C1" s="504"/>
+      <c r="D1" s="504"/>
+      <c r="E1" s="504"/>
+      <c r="F1" s="504"/>
+      <c r="G1" s="504"/>
+      <c r="H1" s="504"/>
+      <c r="I1" s="504"/>
+      <c r="J1" s="504"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -24856,22 +24913,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="481" t="s">
+      <c r="W1" s="505" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="482"/>
+      <c r="X1" s="506"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="480"/>
-      <c r="B2" s="480"/>
-      <c r="C2" s="480"/>
-      <c r="D2" s="480"/>
-      <c r="E2" s="480"/>
-      <c r="F2" s="480"/>
-      <c r="G2" s="480"/>
-      <c r="H2" s="480"/>
-      <c r="I2" s="480"/>
-      <c r="J2" s="480"/>
+      <c r="A2" s="504"/>
+      <c r="B2" s="504"/>
+      <c r="C2" s="504"/>
+      <c r="D2" s="504"/>
+      <c r="E2" s="504"/>
+      <c r="F2" s="504"/>
+      <c r="G2" s="504"/>
+      <c r="H2" s="504"/>
+      <c r="I2" s="504"/>
+      <c r="J2" s="504"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -24925,10 +24982,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="483" t="s">
+      <c r="O3" s="507" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="484"/>
+      <c r="P3" s="508"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -28070,7 +28127,7 @@
       <c r="B55" s="438" t="s">
         <v>24</v>
       </c>
-      <c r="C55" s="499" t="s">
+      <c r="C55" s="490" t="s">
         <v>229</v>
       </c>
       <c r="D55" s="439"/>
@@ -28081,7 +28138,7 @@
       <c r="G55" s="152">
         <v>44627</v>
       </c>
-      <c r="H55" s="528" t="s">
+      <c r="H55" s="530" t="s">
         <v>230</v>
       </c>
       <c r="I55" s="151">
@@ -28100,10 +28157,10 @@
         <f t="shared" si="1"/>
         <v>18886.399999999998</v>
       </c>
-      <c r="O55" s="505" t="s">
+      <c r="O55" s="486" t="s">
         <v>59</v>
       </c>
-      <c r="P55" s="511">
+      <c r="P55" s="480">
         <v>44645</v>
       </c>
       <c r="Q55" s="128"/>
@@ -28114,11 +28171,11 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="527"/>
+      <c r="A56" s="529"/>
       <c r="B56" s="438" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="500"/>
+      <c r="C56" s="491"/>
       <c r="D56" s="440"/>
       <c r="E56" s="60"/>
       <c r="F56" s="151">
@@ -28127,7 +28184,7 @@
       <c r="G56" s="152">
         <v>44627</v>
       </c>
-      <c r="H56" s="529"/>
+      <c r="H56" s="531"/>
       <c r="I56" s="151">
         <v>967</v>
       </c>
@@ -28144,8 +28201,8 @@
         <f t="shared" si="1"/>
         <v>92832</v>
       </c>
-      <c r="O56" s="506"/>
-      <c r="P56" s="512"/>
+      <c r="O56" s="487"/>
+      <c r="P56" s="481"/>
       <c r="Q56" s="164"/>
       <c r="R56" s="158"/>
       <c r="S56" s="92"/>
@@ -28206,13 +28263,13 @@
       <c r="V57" s="54"/>
     </row>
     <row r="58" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="489" t="s">
+      <c r="A58" s="513" t="s">
         <v>41</v>
       </c>
       <c r="B58" s="170" t="s">
         <v>24</v>
       </c>
-      <c r="C58" s="538" t="s">
+      <c r="C58" s="527" t="s">
         <v>319</v>
       </c>
       <c r="D58" s="165"/>
@@ -28223,7 +28280,7 @@
       <c r="G58" s="152">
         <v>44648</v>
       </c>
-      <c r="H58" s="536" t="s">
+      <c r="H58" s="538" t="s">
         <v>315</v>
       </c>
       <c r="I58" s="151">
@@ -28242,10 +28299,10 @@
         <f t="shared" si="1"/>
         <v>35255.600000000006</v>
       </c>
-      <c r="O58" s="493" t="s">
+      <c r="O58" s="494" t="s">
         <v>59</v>
       </c>
-      <c r="P58" s="495">
+      <c r="P58" s="515">
         <v>44662</v>
       </c>
       <c r="Q58" s="164"/>
@@ -28256,11 +28313,11 @@
       <c r="V58" s="54"/>
     </row>
     <row r="59" spans="1:24" s="161" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="490"/>
+      <c r="A59" s="514"/>
       <c r="B59" s="170" t="s">
         <v>23</v>
       </c>
-      <c r="C59" s="539"/>
+      <c r="C59" s="528"/>
       <c r="D59" s="163"/>
       <c r="E59" s="60"/>
       <c r="F59" s="151">
@@ -28269,7 +28326,7 @@
       <c r="G59" s="152">
         <v>44648</v>
       </c>
-      <c r="H59" s="537"/>
+      <c r="H59" s="539"/>
       <c r="I59" s="151">
         <v>719</v>
       </c>
@@ -28286,8 +28343,8 @@
         <f t="shared" si="1"/>
         <v>69024</v>
       </c>
-      <c r="O59" s="494"/>
-      <c r="P59" s="496"/>
+      <c r="O59" s="495"/>
+      <c r="P59" s="516"/>
       <c r="Q59" s="164"/>
       <c r="R59" s="158"/>
       <c r="S59" s="92"/>
@@ -28360,13 +28417,13 @@
       <c r="V61" s="54"/>
     </row>
     <row r="62" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A62" s="530" t="s">
+      <c r="A62" s="532" t="s">
         <v>106</v>
       </c>
       <c r="B62" s="178" t="s">
         <v>237</v>
       </c>
-      <c r="C62" s="532" t="s">
+      <c r="C62" s="534" t="s">
         <v>238</v>
       </c>
       <c r="D62" s="168"/>
@@ -28377,7 +28434,7 @@
       <c r="G62" s="152">
         <v>44622</v>
       </c>
-      <c r="H62" s="534">
+      <c r="H62" s="536">
         <v>37162</v>
       </c>
       <c r="I62" s="151">
@@ -28396,10 +28453,10 @@
         <f t="shared" si="1"/>
         <v>7782.5999999999995</v>
       </c>
-      <c r="O62" s="505" t="s">
+      <c r="O62" s="486" t="s">
         <v>61</v>
       </c>
-      <c r="P62" s="511">
+      <c r="P62" s="480">
         <v>44643</v>
       </c>
       <c r="Q62" s="164"/>
@@ -28410,11 +28467,11 @@
       <c r="V62" s="54"/>
     </row>
     <row r="63" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A63" s="531"/>
+      <c r="A63" s="533"/>
       <c r="B63" s="178" t="s">
         <v>239</v>
       </c>
-      <c r="C63" s="533"/>
+      <c r="C63" s="535"/>
       <c r="D63" s="168"/>
       <c r="E63" s="60"/>
       <c r="F63" s="151">
@@ -28423,7 +28480,7 @@
       <c r="G63" s="152">
         <v>44622</v>
       </c>
-      <c r="H63" s="535"/>
+      <c r="H63" s="537"/>
       <c r="I63" s="151">
         <v>204.8</v>
       </c>
@@ -28440,8 +28497,8 @@
         <f t="shared" si="1"/>
         <v>16998.400000000001</v>
       </c>
-      <c r="O63" s="506"/>
-      <c r="P63" s="512"/>
+      <c r="O63" s="487"/>
+      <c r="P63" s="481"/>
       <c r="Q63" s="164"/>
       <c r="R63" s="129"/>
       <c r="S63" s="92"/>
@@ -28920,8 +28977,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="505"/>
-      <c r="P79" s="507"/>
+      <c r="O79" s="486"/>
+      <c r="P79" s="500"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -28950,8 +29007,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="506"/>
-      <c r="P80" s="508"/>
+      <c r="O80" s="487"/>
+      <c r="P80" s="501"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -28980,8 +29037,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="505"/>
-      <c r="P81" s="507"/>
+      <c r="O81" s="486"/>
+      <c r="P81" s="500"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -29013,8 +29070,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="506"/>
-      <c r="P82" s="508"/>
+      <c r="O82" s="487"/>
+      <c r="P82" s="501"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -29172,8 +29229,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="509"/>
-      <c r="M87" s="510"/>
+      <c r="L87" s="502"/>
+      <c r="M87" s="503"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -29205,8 +29262,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="509"/>
-      <c r="M88" s="510"/>
+      <c r="L88" s="502"/>
+      <c r="M88" s="503"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -29409,8 +29466,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="505"/>
-      <c r="P94" s="501"/>
+      <c r="O94" s="486"/>
+      <c r="P94" s="496"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -29442,8 +29499,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="506"/>
-      <c r="P95" s="502"/>
+      <c r="O95" s="487"/>
+      <c r="P95" s="497"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -34835,11 +34892,11 @@
         <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="503" t="s">
+      <c r="F259" s="498" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="503"/>
-      <c r="H259" s="504"/>
+      <c r="G259" s="498"/>
+      <c r="H259" s="499"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>517031.52999999991</v>
@@ -35413,17 +35470,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="O58:O59"/>
-    <mergeCell ref="P58:P59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O79:O80"/>
-    <mergeCell ref="P79:P80"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="S1:T2"/>
     <mergeCell ref="W1:X1"/>
@@ -35440,6 +35486,17 @@
     <mergeCell ref="O62:O63"/>
     <mergeCell ref="P62:P63"/>
     <mergeCell ref="H58:H59"/>
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O79:O80"/>
+    <mergeCell ref="P79:P80"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="O58:O59"/>
+    <mergeCell ref="P58:P59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -35454,10 +35511,10 @@
   <dimension ref="A1:X292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="3" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="3" topLeftCell="Q53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="Q63" sqref="Q63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -35465,8 +35522,8 @@
     <col min="1" max="1" width="49.28515625" customWidth="1"/>
     <col min="2" max="2" width="28.5703125" style="310" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" style="310" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="310" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="331" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="310" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="331" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" style="311" customWidth="1"/>
     <col min="7" max="7" width="14.140625" style="312" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" style="315" customWidth="1"/>
@@ -35486,18 +35543,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="480" t="s">
+      <c r="A1" s="504" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="480"/>
-      <c r="C1" s="480"/>
-      <c r="D1" s="480"/>
-      <c r="E1" s="480"/>
-      <c r="F1" s="480"/>
-      <c r="G1" s="480"/>
-      <c r="H1" s="480"/>
-      <c r="I1" s="480"/>
-      <c r="J1" s="480"/>
+      <c r="B1" s="504"/>
+      <c r="C1" s="504"/>
+      <c r="D1" s="504"/>
+      <c r="E1" s="504"/>
+      <c r="F1" s="504"/>
+      <c r="G1" s="504"/>
+      <c r="H1" s="504"/>
+      <c r="I1" s="504"/>
+      <c r="J1" s="504"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -35513,22 +35570,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="481" t="s">
+      <c r="W1" s="505" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="482"/>
+      <c r="X1" s="506"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="480"/>
-      <c r="B2" s="480"/>
-      <c r="C2" s="480"/>
-      <c r="D2" s="480"/>
-      <c r="E2" s="480"/>
-      <c r="F2" s="480"/>
-      <c r="G2" s="480"/>
-      <c r="H2" s="480"/>
-      <c r="I2" s="480"/>
-      <c r="J2" s="480"/>
+      <c r="A2" s="504"/>
+      <c r="B2" s="504"/>
+      <c r="C2" s="504"/>
+      <c r="D2" s="504"/>
+      <c r="E2" s="504"/>
+      <c r="F2" s="504"/>
+      <c r="G2" s="504"/>
+      <c r="H2" s="504"/>
+      <c r="I2" s="504"/>
+      <c r="J2" s="504"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -35582,10 +35639,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="483" t="s">
+      <c r="O3" s="507" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="484"/>
+      <c r="P3" s="508"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -36249,18 +36306,22 @@
       <c r="W13" s="53"/>
       <c r="X13" s="70"/>
     </row>
-    <row r="14" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="71" t="s">
         <v>295</v>
       </c>
       <c r="B14" s="58" t="s">
         <v>290</v>
       </c>
-      <c r="C14" s="59"/>
-      <c r="D14" s="60"/>
+      <c r="C14" s="59" t="s">
+        <v>372</v>
+      </c>
+      <c r="D14" s="60">
+        <v>50</v>
+      </c>
       <c r="E14" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1133000</v>
       </c>
       <c r="F14" s="61">
         <v>22660</v>
@@ -36268,7 +36329,9 @@
       <c r="G14" s="62">
         <v>44661</v>
       </c>
-      <c r="H14" s="410"/>
+      <c r="H14" s="410" t="s">
+        <v>386</v>
+      </c>
       <c r="I14" s="411">
         <v>22455</v>
       </c>
@@ -36285,8 +36348,12 @@
         <f t="shared" si="1"/>
         <v>797152.5</v>
       </c>
-      <c r="O14" s="397"/>
-      <c r="P14" s="398"/>
+      <c r="O14" s="397" t="s">
+        <v>61</v>
+      </c>
+      <c r="P14" s="398">
+        <v>44676</v>
+      </c>
       <c r="Q14" s="66">
         <v>26793</v>
       </c>
@@ -36300,15 +36367,19 @@
       <c r="W14" s="53"/>
       <c r="X14" s="70"/>
     </row>
-    <row r="15" spans="1:24" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="73" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="58" t="s">
         <v>296</v>
       </c>
-      <c r="C15" s="59"/>
-      <c r="D15" s="60"/>
+      <c r="C15" s="59" t="s">
+        <v>372</v>
+      </c>
+      <c r="D15" s="60">
+        <v>0</v>
+      </c>
       <c r="E15" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -36319,7 +36390,9 @@
       <c r="G15" s="62">
         <v>44661</v>
       </c>
-      <c r="H15" s="410"/>
+      <c r="H15" s="410" t="s">
+        <v>385</v>
+      </c>
       <c r="I15" s="411">
         <v>6355</v>
       </c>
@@ -36336,8 +36409,12 @@
         <f t="shared" si="1"/>
         <v>225602.5</v>
       </c>
-      <c r="O15" s="397"/>
-      <c r="P15" s="398"/>
+      <c r="O15" s="397" t="s">
+        <v>61</v>
+      </c>
+      <c r="P15" s="398">
+        <v>44676</v>
+      </c>
       <c r="Q15" s="66">
         <v>0</v>
       </c>
@@ -36358,11 +36435,15 @@
       <c r="B16" s="58" t="s">
         <v>298</v>
       </c>
-      <c r="C16" s="74"/>
-      <c r="D16" s="60"/>
+      <c r="C16" s="74" t="s">
+        <v>373</v>
+      </c>
+      <c r="D16" s="60">
+        <v>50</v>
+      </c>
       <c r="E16" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1071000</v>
       </c>
       <c r="F16" s="61">
         <v>21420</v>
@@ -36370,7 +36451,9 @@
       <c r="G16" s="62">
         <v>44662</v>
       </c>
-      <c r="H16" s="410"/>
+      <c r="H16" s="410" t="s">
+        <v>387</v>
+      </c>
       <c r="I16" s="411">
         <v>21410</v>
       </c>
@@ -36387,8 +36470,12 @@
         <f t="shared" si="1"/>
         <v>760055</v>
       </c>
-      <c r="O16" s="397"/>
-      <c r="P16" s="398"/>
+      <c r="O16" s="397" t="s">
+        <v>61</v>
+      </c>
+      <c r="P16" s="398">
+        <v>44676</v>
+      </c>
       <c r="Q16" s="66">
         <v>26686</v>
       </c>
@@ -36402,15 +36489,19 @@
       <c r="W16" s="53"/>
       <c r="X16" s="70"/>
     </row>
-    <row r="17" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="75" t="s">
         <v>223</v>
       </c>
       <c r="B17" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="59"/>
-      <c r="D17" s="60"/>
+      <c r="C17" s="59" t="s">
+        <v>373</v>
+      </c>
+      <c r="D17" s="60">
+        <v>0</v>
+      </c>
       <c r="E17" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -36421,13 +36512,16 @@
       <c r="G17" s="62">
         <v>44662</v>
       </c>
-      <c r="H17" s="410"/>
+      <c r="H17" s="410" t="s">
+        <v>388</v>
+      </c>
       <c r="I17" s="411">
-        <v>5815</v>
+        <f>5815-116.3</f>
+        <v>5698.7</v>
       </c>
       <c r="J17" s="45">
         <f t="shared" si="0"/>
-        <v>5815</v>
+        <v>5698.7</v>
       </c>
       <c r="K17" s="76">
         <v>35.5</v>
@@ -36436,10 +36530,14 @@
       <c r="M17" s="65"/>
       <c r="N17" s="48">
         <f t="shared" si="1"/>
-        <v>206432.5</v>
-      </c>
-      <c r="O17" s="397"/>
-      <c r="P17" s="398"/>
+        <v>202303.85</v>
+      </c>
+      <c r="O17" s="397" t="s">
+        <v>61</v>
+      </c>
+      <c r="P17" s="398">
+        <v>44676</v>
+      </c>
       <c r="Q17" s="66">
         <v>0</v>
       </c>
@@ -36460,11 +36558,15 @@
       <c r="B18" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="59"/>
-      <c r="D18" s="60"/>
+      <c r="C18" s="59" t="s">
+        <v>374</v>
+      </c>
+      <c r="D18" s="60">
+        <v>50</v>
+      </c>
       <c r="E18" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>462500</v>
       </c>
       <c r="F18" s="61">
         <v>9250</v>
@@ -36511,11 +36613,15 @@
       <c r="B19" s="58" t="s">
         <v>300</v>
       </c>
-      <c r="C19" s="59"/>
-      <c r="D19" s="60"/>
+      <c r="C19" s="59" t="s">
+        <v>375</v>
+      </c>
+      <c r="D19" s="60">
+        <v>50</v>
+      </c>
       <c r="E19" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1192000</v>
       </c>
       <c r="F19" s="61">
         <v>23840</v>
@@ -36523,7 +36629,9 @@
       <c r="G19" s="62">
         <v>44664</v>
       </c>
-      <c r="H19" s="410"/>
+      <c r="H19" s="410" t="s">
+        <v>383</v>
+      </c>
       <c r="I19" s="411">
         <v>22455</v>
       </c>
@@ -36566,8 +36674,12 @@
       <c r="B20" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="59"/>
-      <c r="D20" s="60"/>
+      <c r="C20" s="59" t="s">
+        <v>375</v>
+      </c>
+      <c r="D20" s="60">
+        <v>0</v>
+      </c>
       <c r="E20" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -36578,7 +36690,9 @@
       <c r="G20" s="62">
         <v>44664</v>
       </c>
-      <c r="H20" s="410"/>
+      <c r="H20" s="410" t="s">
+        <v>383</v>
+      </c>
       <c r="I20" s="411">
         <v>6355</v>
       </c>
@@ -36621,11 +36735,15 @@
       <c r="B21" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="59"/>
-      <c r="D21" s="60"/>
+      <c r="C21" s="59" t="s">
+        <v>376</v>
+      </c>
+      <c r="D21" s="60">
+        <v>50</v>
+      </c>
       <c r="E21" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1145500</v>
       </c>
       <c r="F21" s="61">
         <v>22910</v>
@@ -36633,7 +36751,9 @@
       <c r="G21" s="62">
         <v>44665</v>
       </c>
-      <c r="H21" s="410"/>
+      <c r="H21" s="410" t="s">
+        <v>384</v>
+      </c>
       <c r="I21" s="411">
         <v>22950</v>
       </c>
@@ -36676,8 +36796,12 @@
       <c r="B22" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="59"/>
-      <c r="D22" s="60"/>
+      <c r="C22" s="59" t="s">
+        <v>376</v>
+      </c>
+      <c r="D22" s="60">
+        <v>0</v>
+      </c>
       <c r="E22" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -36688,7 +36812,9 @@
       <c r="G22" s="62">
         <v>44665</v>
       </c>
-      <c r="H22" s="410"/>
+      <c r="H22" s="410" t="s">
+        <v>384</v>
+      </c>
       <c r="I22" s="411">
         <v>5715</v>
       </c>
@@ -36731,25 +36857,31 @@
       <c r="B23" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="59"/>
-      <c r="D23" s="60"/>
+      <c r="C23" s="59" t="s">
+        <v>377</v>
+      </c>
+      <c r="D23" s="60">
+        <v>50</v>
+      </c>
       <c r="E23" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1196500</v>
       </c>
       <c r="F23" s="61">
-        <v>42890</v>
+        <v>23930</v>
       </c>
       <c r="G23" s="62">
         <v>44668</v>
       </c>
-      <c r="H23" s="410"/>
+      <c r="H23" s="410" t="s">
+        <v>379</v>
+      </c>
       <c r="I23" s="411">
         <v>23990</v>
       </c>
       <c r="J23" s="45">
         <f t="shared" si="0"/>
-        <v>-18900</v>
+        <v>60</v>
       </c>
       <c r="K23" s="76">
         <v>35.5</v>
@@ -36762,8 +36894,12 @@
       </c>
       <c r="O23" s="89"/>
       <c r="P23" s="90"/>
-      <c r="Q23" s="79"/>
-      <c r="R23" s="67"/>
+      <c r="Q23" s="79">
+        <v>27007</v>
+      </c>
+      <c r="R23" s="67">
+        <v>44673</v>
+      </c>
       <c r="S23" s="51">
         <v>11200</v>
       </c>
@@ -36782,8 +36918,12 @@
       <c r="B24" s="58" t="s">
         <v>340</v>
       </c>
-      <c r="C24" s="59"/>
-      <c r="D24" s="60"/>
+      <c r="C24" s="59" t="s">
+        <v>377</v>
+      </c>
+      <c r="D24" s="60">
+        <v>0</v>
+      </c>
       <c r="E24" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -36794,7 +36934,9 @@
       <c r="G24" s="62">
         <v>44668</v>
       </c>
-      <c r="H24" s="410"/>
+      <c r="H24" s="410" t="s">
+        <v>379</v>
+      </c>
       <c r="I24" s="411">
         <v>6665</v>
       </c>
@@ -36813,8 +36955,12 @@
       </c>
       <c r="O24" s="397"/>
       <c r="P24" s="90"/>
-      <c r="Q24" s="79"/>
-      <c r="R24" s="67"/>
+      <c r="Q24" s="79">
+        <v>0</v>
+      </c>
+      <c r="R24" s="67">
+        <v>44673</v>
+      </c>
       <c r="S24" s="91">
         <v>0</v>
       </c>
@@ -36831,13 +36977,17 @@
         <v>341</v>
       </c>
       <c r="B25" s="58" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" s="59"/>
-      <c r="D25" s="60"/>
+        <v>40</v>
+      </c>
+      <c r="C25" s="59" t="s">
+        <v>378</v>
+      </c>
+      <c r="D25" s="60">
+        <v>50</v>
+      </c>
       <c r="E25" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1253500</v>
       </c>
       <c r="F25" s="61">
         <v>25070</v>
@@ -36845,7 +36995,9 @@
       <c r="G25" s="62">
         <v>44670</v>
       </c>
-      <c r="H25" s="410"/>
+      <c r="H25" s="410" t="s">
+        <v>380</v>
+      </c>
       <c r="I25" s="411">
         <v>24940</v>
       </c>
@@ -36864,8 +37016,12 @@
       </c>
       <c r="O25" s="89"/>
       <c r="P25" s="90"/>
-      <c r="Q25" s="79"/>
-      <c r="R25" s="67"/>
+      <c r="Q25" s="79">
+        <v>27328</v>
+      </c>
+      <c r="R25" s="67">
+        <v>44673</v>
+      </c>
       <c r="S25" s="51">
         <v>11200</v>
       </c>
@@ -36884,8 +37040,12 @@
       <c r="B26" s="58" t="s">
         <v>296</v>
       </c>
-      <c r="C26" s="59"/>
-      <c r="D26" s="60"/>
+      <c r="C26" s="59" t="s">
+        <v>378</v>
+      </c>
+      <c r="D26" s="60">
+        <v>0</v>
+      </c>
       <c r="E26" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -36896,7 +37056,9 @@
       <c r="G26" s="62">
         <v>44670</v>
       </c>
-      <c r="H26" s="410"/>
+      <c r="H26" s="410" t="s">
+        <v>380</v>
+      </c>
       <c r="I26" s="411">
         <v>6390</v>
       </c>
@@ -36915,8 +37077,12 @@
       </c>
       <c r="O26" s="89"/>
       <c r="P26" s="90"/>
-      <c r="Q26" s="79"/>
-      <c r="R26" s="67"/>
+      <c r="Q26" s="79">
+        <v>0</v>
+      </c>
+      <c r="R26" s="67">
+        <v>44673</v>
+      </c>
       <c r="S26" s="51">
         <v>0</v>
       </c>
@@ -36929,33 +37095,51 @@
       <c r="X26" s="70"/>
     </row>
     <row r="27" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="82"/>
-      <c r="B27" s="58"/>
+      <c r="A27" s="82" t="s">
+        <v>295</v>
+      </c>
+      <c r="B27" s="58" t="s">
+        <v>72</v>
+      </c>
       <c r="C27" s="59"/>
       <c r="D27" s="60"/>
       <c r="E27" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F27" s="61"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="410"/>
-      <c r="I27" s="411"/>
+      <c r="F27" s="61">
+        <v>22550</v>
+      </c>
+      <c r="G27" s="62">
+        <v>44672</v>
+      </c>
+      <c r="H27" s="410" t="s">
+        <v>381</v>
+      </c>
+      <c r="I27" s="411">
+        <v>22650</v>
+      </c>
       <c r="J27" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K27" s="76"/>
+        <v>100</v>
+      </c>
+      <c r="K27" s="76">
+        <v>35.5</v>
+      </c>
       <c r="L27" s="65"/>
       <c r="M27" s="65"/>
       <c r="N27" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>804075</v>
       </c>
       <c r="O27" s="89"/>
       <c r="P27" s="90"/>
-      <c r="Q27" s="79"/>
-      <c r="R27" s="67"/>
+      <c r="Q27" s="79">
+        <v>26793</v>
+      </c>
+      <c r="R27" s="67">
+        <v>44673</v>
+      </c>
       <c r="S27" s="91"/>
       <c r="T27" s="92"/>
       <c r="U27" s="53"/>
@@ -36964,33 +37148,51 @@
       <c r="X27" s="70"/>
     </row>
     <row r="28" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="82"/>
-      <c r="B28" s="58"/>
+      <c r="A28" s="82" t="s">
+        <v>223</v>
+      </c>
+      <c r="B28" s="58" t="s">
+        <v>296</v>
+      </c>
       <c r="C28" s="59"/>
       <c r="D28" s="60"/>
       <c r="E28" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F28" s="61"/>
-      <c r="G28" s="62"/>
-      <c r="H28" s="410"/>
-      <c r="I28" s="411"/>
+      <c r="F28" s="61">
+        <v>0</v>
+      </c>
+      <c r="G28" s="62">
+        <v>44672</v>
+      </c>
+      <c r="H28" s="410" t="s">
+        <v>381</v>
+      </c>
+      <c r="I28" s="411">
+        <v>5655</v>
+      </c>
       <c r="J28" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K28" s="76"/>
+        <v>5655</v>
+      </c>
+      <c r="K28" s="76">
+        <v>35.5</v>
+      </c>
       <c r="L28" s="65"/>
       <c r="M28" s="65"/>
       <c r="N28" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>200752.5</v>
       </c>
       <c r="O28" s="89"/>
       <c r="P28" s="90"/>
-      <c r="Q28" s="66"/>
-      <c r="R28" s="67"/>
+      <c r="Q28" s="66">
+        <v>0</v>
+      </c>
+      <c r="R28" s="67">
+        <v>44673</v>
+      </c>
       <c r="S28" s="91"/>
       <c r="T28" s="92"/>
       <c r="U28" s="53"/>
@@ -36999,33 +37201,51 @@
       <c r="X28" s="70"/>
     </row>
     <row r="29" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="57"/>
-      <c r="B29" s="93"/>
+      <c r="A29" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="93" t="s">
+        <v>72</v>
+      </c>
       <c r="C29" s="59"/>
       <c r="D29" s="60"/>
       <c r="E29" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F29" s="61"/>
-      <c r="G29" s="62"/>
-      <c r="H29" s="410"/>
-      <c r="I29" s="411"/>
+      <c r="F29" s="61">
+        <v>23530</v>
+      </c>
+      <c r="G29" s="62">
+        <v>44673</v>
+      </c>
+      <c r="H29" s="410" t="s">
+        <v>382</v>
+      </c>
+      <c r="I29" s="411">
+        <v>23490</v>
+      </c>
       <c r="J29" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K29" s="76"/>
+        <v>-40</v>
+      </c>
+      <c r="K29" s="76">
+        <v>35.5</v>
+      </c>
       <c r="L29" s="65"/>
       <c r="M29" s="65"/>
       <c r="N29" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>833895</v>
       </c>
       <c r="O29" s="89"/>
       <c r="P29" s="90"/>
-      <c r="Q29" s="456"/>
-      <c r="R29" s="95"/>
+      <c r="Q29" s="456">
+        <v>26900</v>
+      </c>
+      <c r="R29" s="95">
+        <v>44673</v>
+      </c>
       <c r="S29" s="91"/>
       <c r="T29" s="92"/>
       <c r="U29" s="53"/>
@@ -37034,33 +37254,51 @@
       <c r="X29" s="70"/>
     </row>
     <row r="30" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="57"/>
-      <c r="B30" s="93"/>
+      <c r="A30" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="93" t="s">
+        <v>32</v>
+      </c>
       <c r="C30" s="59"/>
       <c r="D30" s="60"/>
       <c r="E30" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F30" s="61"/>
-      <c r="G30" s="62"/>
-      <c r="H30" s="410"/>
-      <c r="I30" s="411"/>
+      <c r="F30" s="61">
+        <v>0</v>
+      </c>
+      <c r="G30" s="62">
+        <v>44673</v>
+      </c>
+      <c r="H30" s="410" t="s">
+        <v>382</v>
+      </c>
+      <c r="I30" s="411">
+        <v>5845</v>
+      </c>
       <c r="J30" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K30" s="76"/>
+        <v>5845</v>
+      </c>
+      <c r="K30" s="76">
+        <v>35.5</v>
+      </c>
       <c r="L30" s="65"/>
       <c r="M30" s="65"/>
       <c r="N30" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>207497.5</v>
       </c>
       <c r="O30" s="89"/>
       <c r="P30" s="90"/>
-      <c r="Q30" s="94"/>
-      <c r="R30" s="95"/>
+      <c r="Q30" s="94">
+        <v>0</v>
+      </c>
+      <c r="R30" s="95">
+        <v>44673</v>
+      </c>
       <c r="S30" s="91"/>
       <c r="T30" s="92"/>
       <c r="U30" s="53"/>
@@ -38206,28 +38444,48 @@
       <c r="V62" s="54"/>
     </row>
     <row r="63" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A63" s="475"/>
-      <c r="B63" s="178"/>
-      <c r="C63" s="476"/>
+      <c r="A63" s="475" t="s">
+        <v>111</v>
+      </c>
+      <c r="B63" s="178" t="s">
+        <v>389</v>
+      </c>
+      <c r="C63" s="476" t="s">
+        <v>390</v>
+      </c>
       <c r="D63" s="168"/>
       <c r="E63" s="60"/>
-      <c r="F63" s="151"/>
-      <c r="G63" s="152"/>
-      <c r="H63" s="477"/>
-      <c r="I63" s="151"/>
+      <c r="F63" s="151">
+        <v>377.6</v>
+      </c>
+      <c r="G63" s="152">
+        <v>44670</v>
+      </c>
+      <c r="H63" s="477">
+        <v>37713</v>
+      </c>
+      <c r="I63" s="151">
+        <v>377.6</v>
+      </c>
       <c r="J63" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K63" s="166"/>
+      <c r="K63" s="166">
+        <v>57</v>
+      </c>
       <c r="L63" s="99"/>
       <c r="M63" s="99"/>
       <c r="N63" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O63" s="164"/>
-      <c r="P63" s="62"/>
+        <v>21523.200000000001</v>
+      </c>
+      <c r="O63" s="164" t="s">
+        <v>61</v>
+      </c>
+      <c r="P63" s="62">
+        <v>44677</v>
+      </c>
       <c r="Q63" s="164"/>
       <c r="R63" s="129"/>
       <c r="S63" s="92"/>
@@ -38706,8 +38964,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="505"/>
-      <c r="P79" s="507"/>
+      <c r="O79" s="486"/>
+      <c r="P79" s="500"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -38736,8 +38994,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="506"/>
-      <c r="P80" s="508"/>
+      <c r="O80" s="487"/>
+      <c r="P80" s="501"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -38766,8 +39024,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="505"/>
-      <c r="P81" s="507"/>
+      <c r="O81" s="486"/>
+      <c r="P81" s="500"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -38799,8 +39057,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="506"/>
-      <c r="P82" s="508"/>
+      <c r="O82" s="487"/>
+      <c r="P82" s="501"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -38958,8 +39216,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="509"/>
-      <c r="M87" s="510"/>
+      <c r="L87" s="502"/>
+      <c r="M87" s="503"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -38991,8 +39249,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="509"/>
-      <c r="M88" s="510"/>
+      <c r="L88" s="502"/>
+      <c r="M88" s="503"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -39195,8 +39453,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="505"/>
-      <c r="P94" s="501"/>
+      <c r="O94" s="486"/>
+      <c r="P94" s="496"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -39228,8 +39486,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="506"/>
-      <c r="P95" s="502"/>
+      <c r="O95" s="487"/>
+      <c r="P95" s="497"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -44621,14 +44879,14 @@
         <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="503" t="s">
+      <c r="F259" s="498" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="503"/>
-      <c r="H259" s="504"/>
+      <c r="G259" s="498"/>
+      <c r="H259" s="499"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
-        <v>345591.51</v>
+        <v>403492.81</v>
       </c>
       <c r="J259" s="318"/>
       <c r="K259" s="314"/>
@@ -44727,12 +44985,12 @@
       <c r="M263" s="336"/>
       <c r="N263" s="337">
         <f>SUM(N4:N262)</f>
-        <v>12514096.213</v>
+        <v>14577710.762999998</v>
       </c>
       <c r="O263" s="338"/>
       <c r="Q263" s="339">
         <f>SUM(Q4:Q262)</f>
-        <v>241030</v>
+        <v>349058</v>
       </c>
       <c r="R263" s="8"/>
       <c r="S263" s="340">
@@ -44787,7 +45045,7 @@
       <c r="M266" s="352"/>
       <c r="N266" s="353">
         <f>V263+S263+Q263+N263+L263</f>
-        <v>12799926.213</v>
+        <v>14971568.762999998</v>
       </c>
       <c r="O266" s="354"/>
       <c r="R266" s="324"/>
@@ -45199,18 +45457,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="L87:M88"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="O79:O80"/>
     <mergeCell ref="P79:P80"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="S1:T2"/>
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="L87:M88"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRE  13 MAY 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #04  ABRIL   2022/ENTRADAS OBRADOR  ABRIL    2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #04  ABRIL   2022/ENTRADAS OBRADOR  ABRIL    2022.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="409">
   <si>
     <t>FECHA DE PAGO</t>
   </si>
@@ -1240,6 +1240,21 @@
   </si>
   <si>
     <t>D-4023</t>
+  </si>
+  <si>
+    <t>0699 Z</t>
+  </si>
+  <si>
+    <t>0712 Z</t>
+  </si>
+  <si>
+    <t>0732 Z</t>
+  </si>
+  <si>
+    <t>0740 Z</t>
+  </si>
+  <si>
+    <t>0759 Z</t>
   </si>
 </sst>
 </file>
@@ -3872,6 +3887,99 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="9" fillId="17" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="19" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="11" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3890,99 +3998,6 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="19" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="11" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4013,43 +4028,43 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="49" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="49" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="4" fontId="32" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="32" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="49" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="49" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4381,18 +4396,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="506" t="s">
+      <c r="A1" s="482" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="506"/>
-      <c r="C1" s="506"/>
-      <c r="D1" s="506"/>
-      <c r="E1" s="506"/>
-      <c r="F1" s="506"/>
-      <c r="G1" s="506"/>
-      <c r="H1" s="506"/>
-      <c r="I1" s="506"/>
-      <c r="J1" s="506"/>
+      <c r="B1" s="482"/>
+      <c r="C1" s="482"/>
+      <c r="D1" s="482"/>
+      <c r="E1" s="482"/>
+      <c r="F1" s="482"/>
+      <c r="G1" s="482"/>
+      <c r="H1" s="482"/>
+      <c r="I1" s="482"/>
+      <c r="J1" s="482"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -4406,22 +4421,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="507" t="s">
+      <c r="W1" s="483" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="508"/>
+      <c r="X1" s="484"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="506"/>
-      <c r="B2" s="506"/>
-      <c r="C2" s="506"/>
-      <c r="D2" s="506"/>
-      <c r="E2" s="506"/>
-      <c r="F2" s="506"/>
-      <c r="G2" s="506"/>
-      <c r="H2" s="506"/>
-      <c r="I2" s="506"/>
-      <c r="J2" s="506"/>
+      <c r="A2" s="482"/>
+      <c r="B2" s="482"/>
+      <c r="C2" s="482"/>
+      <c r="D2" s="482"/>
+      <c r="E2" s="482"/>
+      <c r="F2" s="482"/>
+      <c r="G2" s="482"/>
+      <c r="H2" s="482"/>
+      <c r="I2" s="482"/>
+      <c r="J2" s="482"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -4475,10 +4490,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="509" t="s">
+      <c r="O3" s="485" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="510"/>
+      <c r="P3" s="486"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -5022,7 +5037,7 @@
       <c r="B12" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="511" t="s">
+      <c r="C12" s="487" t="s">
         <v>103</v>
       </c>
       <c r="D12" s="400"/>
@@ -5086,7 +5101,7 @@
       <c r="B13" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="512"/>
+      <c r="C13" s="488"/>
       <c r="D13" s="400"/>
       <c r="E13" s="401"/>
       <c r="F13" s="402">
@@ -7088,13 +7103,13 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="490" t="s">
+      <c r="A56" s="499" t="s">
         <v>41</v>
       </c>
       <c r="B56" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C56" s="492" t="s">
+      <c r="C56" s="501" t="s">
         <v>110</v>
       </c>
       <c r="D56" s="150"/>
@@ -7105,7 +7120,7 @@
       <c r="G56" s="152">
         <v>44571</v>
       </c>
-      <c r="H56" s="494">
+      <c r="H56" s="493">
         <v>782</v>
       </c>
       <c r="I56" s="151">
@@ -7134,11 +7149,11 @@
       <c r="V56" s="160"/>
     </row>
     <row r="57" spans="1:24" s="161" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="491"/>
+      <c r="A57" s="500"/>
       <c r="B57" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="493"/>
+      <c r="C57" s="502"/>
       <c r="D57" s="150"/>
       <c r="E57" s="40"/>
       <c r="F57" s="151">
@@ -7147,7 +7162,7 @@
       <c r="G57" s="152">
         <v>44571</v>
       </c>
-      <c r="H57" s="495"/>
+      <c r="H57" s="494"/>
       <c r="I57" s="151">
         <v>319</v>
       </c>
@@ -7174,13 +7189,13 @@
       <c r="V57" s="160"/>
     </row>
     <row r="58" spans="1:24" s="161" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="490" t="s">
+      <c r="A58" s="499" t="s">
         <v>41</v>
       </c>
       <c r="B58" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="492" t="s">
+      <c r="C58" s="501" t="s">
         <v>129</v>
       </c>
       <c r="D58" s="150"/>
@@ -7191,7 +7206,7 @@
       <c r="G58" s="152">
         <v>44578</v>
       </c>
-      <c r="H58" s="494">
+      <c r="H58" s="493">
         <v>810</v>
       </c>
       <c r="I58" s="151">
@@ -7210,10 +7225,10 @@
         <f t="shared" si="1"/>
         <v>75875.8</v>
       </c>
-      <c r="O58" s="496" t="s">
+      <c r="O58" s="495" t="s">
         <v>59</v>
       </c>
-      <c r="P58" s="517">
+      <c r="P58" s="497">
         <v>44606</v>
       </c>
       <c r="Q58" s="128"/>
@@ -7224,11 +7239,11 @@
       <c r="V58" s="160"/>
     </row>
     <row r="59" spans="1:24" s="161" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="491"/>
+      <c r="A59" s="500"/>
       <c r="B59" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C59" s="493"/>
+      <c r="C59" s="502"/>
       <c r="D59" s="150"/>
       <c r="E59" s="40"/>
       <c r="F59" s="151">
@@ -7237,7 +7252,7 @@
       <c r="G59" s="152">
         <v>44578</v>
       </c>
-      <c r="H59" s="495"/>
+      <c r="H59" s="494"/>
       <c r="I59" s="151">
         <v>220</v>
       </c>
@@ -7254,8 +7269,8 @@
         <f t="shared" si="1"/>
         <v>22440</v>
       </c>
-      <c r="O59" s="497"/>
-      <c r="P59" s="518"/>
+      <c r="O59" s="496"/>
+      <c r="P59" s="498"/>
       <c r="Q59" s="128"/>
       <c r="R59" s="158"/>
       <c r="S59" s="92"/>
@@ -7264,13 +7279,13 @@
       <c r="V59" s="160"/>
     </row>
     <row r="60" spans="1:24" s="161" customFormat="1" ht="48.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="515" t="s">
+      <c r="A60" s="491" t="s">
         <v>41</v>
       </c>
       <c r="B60" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C60" s="513" t="s">
+      <c r="C60" s="489" t="s">
         <v>109</v>
       </c>
       <c r="D60" s="163"/>
@@ -7284,7 +7299,7 @@
       <c r="G60" s="152">
         <v>44585</v>
       </c>
-      <c r="H60" s="494">
+      <c r="H60" s="493">
         <v>800</v>
       </c>
       <c r="I60" s="151">
@@ -7303,10 +7318,10 @@
         <f t="shared" si="1"/>
         <v>151187.4</v>
       </c>
-      <c r="O60" s="496" t="s">
+      <c r="O60" s="495" t="s">
         <v>59</v>
       </c>
-      <c r="P60" s="517">
+      <c r="P60" s="497">
         <v>44594</v>
       </c>
       <c r="Q60" s="164"/>
@@ -7319,11 +7334,11 @@
       <c r="X60"/>
     </row>
     <row r="61" spans="1:24" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="516"/>
+      <c r="A61" s="492"/>
       <c r="B61" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C61" s="514"/>
+      <c r="C61" s="490"/>
       <c r="D61" s="165"/>
       <c r="E61" s="40">
         <f t="shared" si="2"/>
@@ -7335,7 +7350,7 @@
       <c r="G61" s="152">
         <v>44585</v>
       </c>
-      <c r="H61" s="495"/>
+      <c r="H61" s="494"/>
       <c r="I61" s="151">
         <v>231.6</v>
       </c>
@@ -7352,8 +7367,8 @@
         <f t="shared" si="1"/>
         <v>23623.200000000001</v>
       </c>
-      <c r="O61" s="497"/>
-      <c r="P61" s="518"/>
+      <c r="O61" s="496"/>
+      <c r="P61" s="498"/>
       <c r="Q61" s="164"/>
       <c r="R61" s="129"/>
       <c r="S61" s="92"/>
@@ -7419,7 +7434,7 @@
       <c r="B63" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C63" s="484"/>
+      <c r="C63" s="515"/>
       <c r="D63" s="163"/>
       <c r="E63" s="40">
         <f t="shared" si="2"/>
@@ -7427,7 +7442,7 @@
       </c>
       <c r="F63" s="151"/>
       <c r="G63" s="152"/>
-      <c r="H63" s="486"/>
+      <c r="H63" s="517"/>
       <c r="I63" s="151"/>
       <c r="J63" s="45">
         <f t="shared" si="0"/>
@@ -7456,7 +7471,7 @@
       <c r="B64" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C64" s="485"/>
+      <c r="C64" s="516"/>
       <c r="D64" s="168"/>
       <c r="E64" s="40">
         <f t="shared" si="2"/>
@@ -7464,7 +7479,7 @@
       </c>
       <c r="F64" s="151"/>
       <c r="G64" s="152"/>
-      <c r="H64" s="487"/>
+      <c r="H64" s="518"/>
       <c r="I64" s="151"/>
       <c r="J64" s="45">
         <f t="shared" si="0"/>
@@ -7642,8 +7657,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O68" s="488"/>
-      <c r="P68" s="482"/>
+      <c r="O68" s="507"/>
+      <c r="P68" s="513"/>
       <c r="Q68" s="164"/>
       <c r="R68" s="129"/>
       <c r="S68" s="180"/>
@@ -7677,8 +7692,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O69" s="489"/>
-      <c r="P69" s="483"/>
+      <c r="O69" s="508"/>
+      <c r="P69" s="514"/>
       <c r="Q69" s="164"/>
       <c r="R69" s="129"/>
       <c r="S69" s="180"/>
@@ -8168,8 +8183,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="488"/>
-      <c r="P82" s="502"/>
+      <c r="O82" s="507"/>
+      <c r="P82" s="509"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="129"/>
       <c r="S82" s="180"/>
@@ -8201,8 +8216,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O83" s="489"/>
-      <c r="P83" s="503"/>
+      <c r="O83" s="508"/>
+      <c r="P83" s="510"/>
       <c r="Q83" s="164"/>
       <c r="R83" s="129"/>
       <c r="S83" s="180"/>
@@ -8234,8 +8249,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O84" s="488"/>
-      <c r="P84" s="502"/>
+      <c r="O84" s="507"/>
+      <c r="P84" s="509"/>
       <c r="Q84" s="164"/>
       <c r="R84" s="158"/>
       <c r="S84" s="180"/>
@@ -8267,8 +8282,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O85" s="489"/>
-      <c r="P85" s="503"/>
+      <c r="O85" s="508"/>
+      <c r="P85" s="510"/>
       <c r="Q85" s="164"/>
       <c r="R85" s="158"/>
       <c r="S85" s="180"/>
@@ -8426,8 +8441,8 @@
         <v>0</v>
       </c>
       <c r="K90" s="100"/>
-      <c r="L90" s="504"/>
-      <c r="M90" s="505"/>
+      <c r="L90" s="511"/>
+      <c r="M90" s="512"/>
       <c r="N90" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8459,8 +8474,8 @@
         <v>0</v>
       </c>
       <c r="K91" s="100"/>
-      <c r="L91" s="504"/>
-      <c r="M91" s="505"/>
+      <c r="L91" s="511"/>
+      <c r="M91" s="512"/>
       <c r="N91" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8663,8 +8678,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O97" s="488"/>
-      <c r="P97" s="498"/>
+      <c r="O97" s="507"/>
+      <c r="P97" s="503"/>
       <c r="Q97" s="164"/>
       <c r="R97" s="129"/>
       <c r="S97" s="180"/>
@@ -8696,8 +8711,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O98" s="489"/>
-      <c r="P98" s="499"/>
+      <c r="O98" s="508"/>
+      <c r="P98" s="504"/>
       <c r="Q98" s="164"/>
       <c r="R98" s="129"/>
       <c r="S98" s="180"/>
@@ -14089,11 +14104,11 @@
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F262" s="500" t="s">
+      <c r="F262" s="505" t="s">
         <v>26</v>
       </c>
-      <c r="G262" s="500"/>
-      <c r="H262" s="501"/>
+      <c r="G262" s="505"/>
+      <c r="H262" s="506"/>
       <c r="I262" s="317">
         <f>SUM(I4:I261)</f>
         <v>426245.47000000003</v>
@@ -14667,6 +14682,22 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="P68:P69"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="H63:H64"/>
+    <mergeCell ref="O68:O69"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="O58:O59"/>
+    <mergeCell ref="P97:P98"/>
+    <mergeCell ref="F262:H262"/>
+    <mergeCell ref="O82:O83"/>
+    <mergeCell ref="P82:P83"/>
+    <mergeCell ref="O84:O85"/>
+    <mergeCell ref="P84:P85"/>
+    <mergeCell ref="L90:M91"/>
+    <mergeCell ref="O97:O98"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="O3:P3"/>
@@ -14680,22 +14711,6 @@
     <mergeCell ref="C56:C57"/>
     <mergeCell ref="H56:H57"/>
     <mergeCell ref="P58:P59"/>
-    <mergeCell ref="P97:P98"/>
-    <mergeCell ref="F262:H262"/>
-    <mergeCell ref="O82:O83"/>
-    <mergeCell ref="P82:P83"/>
-    <mergeCell ref="O84:O85"/>
-    <mergeCell ref="P84:P85"/>
-    <mergeCell ref="L90:M91"/>
-    <mergeCell ref="O97:O98"/>
-    <mergeCell ref="P68:P69"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="O68:O69"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="H58:H59"/>
-    <mergeCell ref="O58:O59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -14739,18 +14754,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="506" t="s">
+      <c r="A1" s="482" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="506"/>
-      <c r="C1" s="506"/>
-      <c r="D1" s="506"/>
-      <c r="E1" s="506"/>
-      <c r="F1" s="506"/>
-      <c r="G1" s="506"/>
-      <c r="H1" s="506"/>
-      <c r="I1" s="506"/>
-      <c r="J1" s="506"/>
+      <c r="B1" s="482"/>
+      <c r="C1" s="482"/>
+      <c r="D1" s="482"/>
+      <c r="E1" s="482"/>
+      <c r="F1" s="482"/>
+      <c r="G1" s="482"/>
+      <c r="H1" s="482"/>
+      <c r="I1" s="482"/>
+      <c r="J1" s="482"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -14766,22 +14781,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="507" t="s">
+      <c r="W1" s="483" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="508"/>
+      <c r="X1" s="484"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="506"/>
-      <c r="B2" s="506"/>
-      <c r="C2" s="506"/>
-      <c r="D2" s="506"/>
-      <c r="E2" s="506"/>
-      <c r="F2" s="506"/>
-      <c r="G2" s="506"/>
-      <c r="H2" s="506"/>
-      <c r="I2" s="506"/>
-      <c r="J2" s="506"/>
+      <c r="A2" s="482"/>
+      <c r="B2" s="482"/>
+      <c r="C2" s="482"/>
+      <c r="D2" s="482"/>
+      <c r="E2" s="482"/>
+      <c r="F2" s="482"/>
+      <c r="G2" s="482"/>
+      <c r="H2" s="482"/>
+      <c r="I2" s="482"/>
+      <c r="J2" s="482"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -14835,10 +14850,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="509" t="s">
+      <c r="O3" s="485" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="510"/>
+      <c r="P3" s="486"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -17480,7 +17495,7 @@
       <c r="B55" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C55" s="492" t="s">
+      <c r="C55" s="501" t="s">
         <v>160</v>
       </c>
       <c r="D55" s="150"/>
@@ -17491,7 +17506,7 @@
       <c r="G55" s="152">
         <v>44599</v>
       </c>
-      <c r="H55" s="486" t="s">
+      <c r="H55" s="517" t="s">
         <v>161</v>
       </c>
       <c r="I55" s="151">
@@ -17524,7 +17539,7 @@
       <c r="B56" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="493"/>
+      <c r="C56" s="502"/>
       <c r="D56" s="163"/>
       <c r="E56" s="40"/>
       <c r="F56" s="151">
@@ -17533,7 +17548,7 @@
       <c r="G56" s="152">
         <v>44599</v>
       </c>
-      <c r="H56" s="487"/>
+      <c r="H56" s="518"/>
       <c r="I56" s="151">
         <v>194.4</v>
       </c>
@@ -17579,7 +17594,7 @@
       <c r="G57" s="152">
         <v>44606</v>
       </c>
-      <c r="H57" s="486" t="s">
+      <c r="H57" s="517" t="s">
         <v>163</v>
       </c>
       <c r="I57" s="151">
@@ -17598,10 +17613,10 @@
         <f t="shared" si="1"/>
         <v>35776</v>
       </c>
-      <c r="O57" s="488" t="s">
+      <c r="O57" s="507" t="s">
         <v>59</v>
       </c>
-      <c r="P57" s="482">
+      <c r="P57" s="513">
         <v>44620</v>
       </c>
       <c r="Q57" s="164"/>
@@ -17625,7 +17640,7 @@
       <c r="G58" s="152">
         <v>44606</v>
       </c>
-      <c r="H58" s="487"/>
+      <c r="H58" s="518"/>
       <c r="I58" s="151">
         <v>627.60209999999995</v>
       </c>
@@ -17669,7 +17684,7 @@
       <c r="G59" s="152">
         <v>44613</v>
       </c>
-      <c r="H59" s="486" t="s">
+      <c r="H59" s="517" t="s">
         <v>225</v>
       </c>
       <c r="I59" s="151">
@@ -17713,7 +17728,7 @@
       <c r="E60" s="40"/>
       <c r="F60" s="151"/>
       <c r="G60" s="152"/>
-      <c r="H60" s="487"/>
+      <c r="H60" s="518"/>
       <c r="I60" s="151"/>
       <c r="J60" s="45">
         <f t="shared" si="0"/>
@@ -18376,8 +18391,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="488"/>
-      <c r="P79" s="502"/>
+      <c r="O79" s="507"/>
+      <c r="P79" s="509"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -18406,8 +18421,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="489"/>
-      <c r="P80" s="503"/>
+      <c r="O80" s="508"/>
+      <c r="P80" s="510"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -18436,8 +18451,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="488"/>
-      <c r="P81" s="502"/>
+      <c r="O81" s="507"/>
+      <c r="P81" s="509"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -18469,8 +18484,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="489"/>
-      <c r="P82" s="503"/>
+      <c r="O82" s="508"/>
+      <c r="P82" s="510"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -18628,8 +18643,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="504"/>
-      <c r="M87" s="505"/>
+      <c r="L87" s="511"/>
+      <c r="M87" s="512"/>
       <c r="N87" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -18661,8 +18676,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="504"/>
-      <c r="M88" s="505"/>
+      <c r="L88" s="511"/>
+      <c r="M88" s="512"/>
       <c r="N88" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -18865,8 +18880,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="488"/>
-      <c r="P94" s="498"/>
+      <c r="O94" s="507"/>
+      <c r="P94" s="503"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -18898,8 +18913,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="489"/>
-      <c r="P95" s="499"/>
+      <c r="O95" s="508"/>
+      <c r="P95" s="504"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -24291,11 +24306,11 @@
         <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="500" t="s">
+      <c r="F259" s="505" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="500"/>
-      <c r="H259" s="501"/>
+      <c r="G259" s="505"/>
+      <c r="H259" s="506"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>387207.97210000001</v>
@@ -24869,12 +24884,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="L87:M88"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
     <mergeCell ref="O79:O80"/>
     <mergeCell ref="P79:P80"/>
     <mergeCell ref="A1:J2"/>
@@ -24890,6 +24899,12 @@
     <mergeCell ref="C55:C56"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="H55:H56"/>
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="L87:M88"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -24936,18 +24951,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="506" t="s">
+      <c r="A1" s="482" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="506"/>
-      <c r="C1" s="506"/>
-      <c r="D1" s="506"/>
-      <c r="E1" s="506"/>
-      <c r="F1" s="506"/>
-      <c r="G1" s="506"/>
-      <c r="H1" s="506"/>
-      <c r="I1" s="506"/>
-      <c r="J1" s="506"/>
+      <c r="B1" s="482"/>
+      <c r="C1" s="482"/>
+      <c r="D1" s="482"/>
+      <c r="E1" s="482"/>
+      <c r="F1" s="482"/>
+      <c r="G1" s="482"/>
+      <c r="H1" s="482"/>
+      <c r="I1" s="482"/>
+      <c r="J1" s="482"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -24963,22 +24978,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="507" t="s">
+      <c r="W1" s="483" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="508"/>
+      <c r="X1" s="484"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="506"/>
-      <c r="B2" s="506"/>
-      <c r="C2" s="506"/>
-      <c r="D2" s="506"/>
-      <c r="E2" s="506"/>
-      <c r="F2" s="506"/>
-      <c r="G2" s="506"/>
-      <c r="H2" s="506"/>
-      <c r="I2" s="506"/>
-      <c r="J2" s="506"/>
+      <c r="A2" s="482"/>
+      <c r="B2" s="482"/>
+      <c r="C2" s="482"/>
+      <c r="D2" s="482"/>
+      <c r="E2" s="482"/>
+      <c r="F2" s="482"/>
+      <c r="G2" s="482"/>
+      <c r="H2" s="482"/>
+      <c r="I2" s="482"/>
+      <c r="J2" s="482"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -25032,10 +25047,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="509" t="s">
+      <c r="O3" s="485" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="510"/>
+      <c r="P3" s="486"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -28249,7 +28264,7 @@
       <c r="B55" s="438" t="s">
         <v>24</v>
       </c>
-      <c r="C55" s="492" t="s">
+      <c r="C55" s="501" t="s">
         <v>229</v>
       </c>
       <c r="D55" s="439"/>
@@ -28260,7 +28275,7 @@
       <c r="G55" s="152">
         <v>44627</v>
       </c>
-      <c r="H55" s="532" t="s">
+      <c r="H55" s="530" t="s">
         <v>230</v>
       </c>
       <c r="I55" s="151">
@@ -28279,10 +28294,10 @@
         <f t="shared" si="1"/>
         <v>18886.399999999998</v>
       </c>
-      <c r="O55" s="488" t="s">
+      <c r="O55" s="507" t="s">
         <v>59</v>
       </c>
-      <c r="P55" s="482">
+      <c r="P55" s="513">
         <v>44645</v>
       </c>
       <c r="Q55" s="128"/>
@@ -28293,11 +28308,11 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="531"/>
+      <c r="A56" s="529"/>
       <c r="B56" s="438" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="493"/>
+      <c r="C56" s="502"/>
       <c r="D56" s="440"/>
       <c r="E56" s="60"/>
       <c r="F56" s="151">
@@ -28306,7 +28321,7 @@
       <c r="G56" s="152">
         <v>44627</v>
       </c>
-      <c r="H56" s="533"/>
+      <c r="H56" s="531"/>
       <c r="I56" s="151">
         <v>967</v>
       </c>
@@ -28323,8 +28338,8 @@
         <f t="shared" si="1"/>
         <v>92832</v>
       </c>
-      <c r="O56" s="489"/>
-      <c r="P56" s="483"/>
+      <c r="O56" s="508"/>
+      <c r="P56" s="514"/>
       <c r="Q56" s="164"/>
       <c r="R56" s="158"/>
       <c r="S56" s="92"/>
@@ -28385,13 +28400,13 @@
       <c r="V57" s="54"/>
     </row>
     <row r="58" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="515" t="s">
+      <c r="A58" s="491" t="s">
         <v>41</v>
       </c>
       <c r="B58" s="170" t="s">
         <v>24</v>
       </c>
-      <c r="C58" s="529" t="s">
+      <c r="C58" s="540" t="s">
         <v>319</v>
       </c>
       <c r="D58" s="165"/>
@@ -28402,7 +28417,7 @@
       <c r="G58" s="152">
         <v>44648</v>
       </c>
-      <c r="H58" s="540" t="s">
+      <c r="H58" s="538" t="s">
         <v>315</v>
       </c>
       <c r="I58" s="151">
@@ -28421,10 +28436,10 @@
         <f t="shared" si="1"/>
         <v>35255.600000000006</v>
       </c>
-      <c r="O58" s="496" t="s">
+      <c r="O58" s="495" t="s">
         <v>59</v>
       </c>
-      <c r="P58" s="517">
+      <c r="P58" s="497">
         <v>44662</v>
       </c>
       <c r="Q58" s="164"/>
@@ -28435,11 +28450,11 @@
       <c r="V58" s="54"/>
     </row>
     <row r="59" spans="1:24" s="161" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="516"/>
+      <c r="A59" s="492"/>
       <c r="B59" s="170" t="s">
         <v>23</v>
       </c>
-      <c r="C59" s="530"/>
+      <c r="C59" s="541"/>
       <c r="D59" s="163"/>
       <c r="E59" s="60"/>
       <c r="F59" s="151">
@@ -28448,7 +28463,7 @@
       <c r="G59" s="152">
         <v>44648</v>
       </c>
-      <c r="H59" s="541"/>
+      <c r="H59" s="539"/>
       <c r="I59" s="151">
         <v>719</v>
       </c>
@@ -28465,8 +28480,8 @@
         <f t="shared" si="1"/>
         <v>69024</v>
       </c>
-      <c r="O59" s="497"/>
-      <c r="P59" s="518"/>
+      <c r="O59" s="496"/>
+      <c r="P59" s="498"/>
       <c r="Q59" s="164"/>
       <c r="R59" s="158"/>
       <c r="S59" s="92"/>
@@ -28539,13 +28554,13 @@
       <c r="V61" s="54"/>
     </row>
     <row r="62" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A62" s="534" t="s">
+      <c r="A62" s="532" t="s">
         <v>106</v>
       </c>
       <c r="B62" s="178" t="s">
         <v>237</v>
       </c>
-      <c r="C62" s="536" t="s">
+      <c r="C62" s="534" t="s">
         <v>238</v>
       </c>
       <c r="D62" s="168"/>
@@ -28556,7 +28571,7 @@
       <c r="G62" s="152">
         <v>44622</v>
       </c>
-      <c r="H62" s="538">
+      <c r="H62" s="536">
         <v>37162</v>
       </c>
       <c r="I62" s="151">
@@ -28575,10 +28590,10 @@
         <f t="shared" si="1"/>
         <v>7782.5999999999995</v>
       </c>
-      <c r="O62" s="488" t="s">
+      <c r="O62" s="507" t="s">
         <v>61</v>
       </c>
-      <c r="P62" s="482">
+      <c r="P62" s="513">
         <v>44643</v>
       </c>
       <c r="Q62" s="164"/>
@@ -28589,11 +28604,11 @@
       <c r="V62" s="54"/>
     </row>
     <row r="63" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A63" s="535"/>
+      <c r="A63" s="533"/>
       <c r="B63" s="178" t="s">
         <v>239</v>
       </c>
-      <c r="C63" s="537"/>
+      <c r="C63" s="535"/>
       <c r="D63" s="168"/>
       <c r="E63" s="60"/>
       <c r="F63" s="151">
@@ -28602,7 +28617,7 @@
       <c r="G63" s="152">
         <v>44622</v>
       </c>
-      <c r="H63" s="539"/>
+      <c r="H63" s="537"/>
       <c r="I63" s="151">
         <v>204.8</v>
       </c>
@@ -28619,8 +28634,8 @@
         <f t="shared" si="1"/>
         <v>16998.400000000001</v>
       </c>
-      <c r="O63" s="489"/>
-      <c r="P63" s="483"/>
+      <c r="O63" s="508"/>
+      <c r="P63" s="514"/>
       <c r="Q63" s="164"/>
       <c r="R63" s="129"/>
       <c r="S63" s="92"/>
@@ -29099,8 +29114,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="488"/>
-      <c r="P79" s="502"/>
+      <c r="O79" s="507"/>
+      <c r="P79" s="509"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -29129,8 +29144,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="489"/>
-      <c r="P80" s="503"/>
+      <c r="O80" s="508"/>
+      <c r="P80" s="510"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -29159,8 +29174,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="488"/>
-      <c r="P81" s="502"/>
+      <c r="O81" s="507"/>
+      <c r="P81" s="509"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -29192,8 +29207,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="489"/>
-      <c r="P82" s="503"/>
+      <c r="O82" s="508"/>
+      <c r="P82" s="510"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -29351,8 +29366,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="504"/>
-      <c r="M87" s="505"/>
+      <c r="L87" s="511"/>
+      <c r="M87" s="512"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -29384,8 +29399,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="504"/>
-      <c r="M88" s="505"/>
+      <c r="L88" s="511"/>
+      <c r="M88" s="512"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -29588,8 +29603,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="488"/>
-      <c r="P94" s="498"/>
+      <c r="O94" s="507"/>
+      <c r="P94" s="503"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -29621,8 +29636,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="489"/>
-      <c r="P95" s="499"/>
+      <c r="O95" s="508"/>
+      <c r="P95" s="504"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -35014,11 +35029,11 @@
         <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="500" t="s">
+      <c r="F259" s="505" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="500"/>
-      <c r="H259" s="501"/>
+      <c r="G259" s="505"/>
+      <c r="H259" s="506"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>517031.52999999991</v>
@@ -35592,6 +35607,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="O58:O59"/>
+    <mergeCell ref="P58:P59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O79:O80"/>
+    <mergeCell ref="P79:P80"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="S1:T2"/>
     <mergeCell ref="W1:X1"/>
@@ -35608,17 +35634,6 @@
     <mergeCell ref="O62:O63"/>
     <mergeCell ref="P62:P63"/>
     <mergeCell ref="H58:H59"/>
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O79:O80"/>
-    <mergeCell ref="P79:P80"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="O58:O59"/>
-    <mergeCell ref="P58:P59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -35633,10 +35648,10 @@
   <dimension ref="A1:X292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="3" topLeftCell="O15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="3" topLeftCell="O24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O21" sqref="O21"/>
+      <selection pane="bottomRight" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -35644,8 +35659,8 @@
     <col min="1" max="1" width="49.28515625" customWidth="1"/>
     <col min="2" max="2" width="28.5703125" style="310" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" style="310" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="310" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="331" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="310" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="331" customWidth="1"/>
     <col min="6" max="6" width="14.140625" style="311" customWidth="1"/>
     <col min="7" max="7" width="14.140625" style="312" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" style="315" customWidth="1"/>
@@ -35665,18 +35680,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="506" t="s">
+      <c r="A1" s="482" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="506"/>
-      <c r="C1" s="506"/>
-      <c r="D1" s="506"/>
-      <c r="E1" s="506"/>
-      <c r="F1" s="506"/>
-      <c r="G1" s="506"/>
-      <c r="H1" s="506"/>
-      <c r="I1" s="506"/>
-      <c r="J1" s="506"/>
+      <c r="B1" s="482"/>
+      <c r="C1" s="482"/>
+      <c r="D1" s="482"/>
+      <c r="E1" s="482"/>
+      <c r="F1" s="482"/>
+      <c r="G1" s="482"/>
+      <c r="H1" s="482"/>
+      <c r="I1" s="482"/>
+      <c r="J1" s="482"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -35692,22 +35707,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="507" t="s">
+      <c r="W1" s="483" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="508"/>
+      <c r="X1" s="484"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="506"/>
-      <c r="B2" s="506"/>
-      <c r="C2" s="506"/>
-      <c r="D2" s="506"/>
-      <c r="E2" s="506"/>
-      <c r="F2" s="506"/>
-      <c r="G2" s="506"/>
-      <c r="H2" s="506"/>
-      <c r="I2" s="506"/>
-      <c r="J2" s="506"/>
+      <c r="A2" s="482"/>
+      <c r="B2" s="482"/>
+      <c r="C2" s="482"/>
+      <c r="D2" s="482"/>
+      <c r="E2" s="482"/>
+      <c r="F2" s="482"/>
+      <c r="G2" s="482"/>
+      <c r="H2" s="482"/>
+      <c r="I2" s="482"/>
+      <c r="J2" s="482"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -35761,10 +35776,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="509" t="s">
+      <c r="O3" s="485" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="510"/>
+      <c r="P3" s="486"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -37256,11 +37271,15 @@
       <c r="B27" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="59"/>
-      <c r="D27" s="60"/>
+      <c r="C27" s="59" t="s">
+        <v>404</v>
+      </c>
+      <c r="D27" s="60">
+        <v>50</v>
+      </c>
       <c r="E27" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1127500</v>
       </c>
       <c r="F27" s="61">
         <v>22550</v>
@@ -37313,8 +37332,12 @@
       <c r="B28" s="58" t="s">
         <v>296</v>
       </c>
-      <c r="C28" s="59"/>
-      <c r="D28" s="60"/>
+      <c r="C28" s="59" t="s">
+        <v>404</v>
+      </c>
+      <c r="D28" s="60">
+        <v>50</v>
+      </c>
       <c r="E28" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -37370,11 +37393,15 @@
       <c r="B29" s="93" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="59"/>
-      <c r="D29" s="60"/>
+      <c r="C29" s="59" t="s">
+        <v>405</v>
+      </c>
+      <c r="D29" s="60">
+        <v>50</v>
+      </c>
       <c r="E29" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1176500</v>
       </c>
       <c r="F29" s="61">
         <v>23530</v>
@@ -37427,8 +37454,12 @@
       <c r="B30" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="59"/>
-      <c r="D30" s="60"/>
+      <c r="C30" s="59" t="s">
+        <v>405</v>
+      </c>
+      <c r="D30" s="60">
+        <v>50</v>
+      </c>
       <c r="E30" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -37484,11 +37515,15 @@
       <c r="B31" s="93" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="59"/>
-      <c r="D31" s="60"/>
+      <c r="C31" s="59" t="s">
+        <v>406</v>
+      </c>
+      <c r="D31" s="60">
+        <v>50</v>
+      </c>
       <c r="E31" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1212500</v>
       </c>
       <c r="F31" s="61">
         <v>24250</v>
@@ -37537,8 +37572,12 @@
       <c r="B32" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="59"/>
-      <c r="D32" s="60"/>
+      <c r="C32" s="59" t="s">
+        <v>406</v>
+      </c>
+      <c r="D32" s="60">
+        <v>50</v>
+      </c>
       <c r="E32" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -37590,11 +37629,15 @@
       <c r="B33" s="93" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="59"/>
-      <c r="D33" s="60"/>
+      <c r="C33" s="59" t="s">
+        <v>407</v>
+      </c>
+      <c r="D33" s="60">
+        <v>50</v>
+      </c>
       <c r="E33" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1126000</v>
       </c>
       <c r="F33" s="61">
         <v>22520</v>
@@ -37647,8 +37690,12 @@
       <c r="B34" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="59"/>
-      <c r="D34" s="60"/>
+      <c r="C34" s="59" t="s">
+        <v>407</v>
+      </c>
+      <c r="D34" s="60">
+        <v>50</v>
+      </c>
       <c r="E34" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -37704,11 +37751,15 @@
       <c r="B35" s="93" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="59"/>
-      <c r="D35" s="60"/>
+      <c r="C35" s="59" t="s">
+        <v>408</v>
+      </c>
+      <c r="D35" s="60">
+        <v>50</v>
+      </c>
       <c r="E35" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1155260</v>
       </c>
       <c r="F35" s="61">
         <v>23105.200000000001</v>
@@ -37761,7 +37812,9 @@
       <c r="B36" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="59"/>
+      <c r="C36" s="59" t="s">
+        <v>408</v>
+      </c>
       <c r="D36" s="60"/>
       <c r="E36" s="40">
         <f t="shared" si="2"/>
@@ -39259,8 +39312,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="488"/>
-      <c r="P79" s="502"/>
+      <c r="O79" s="507"/>
+      <c r="P79" s="509"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -39289,8 +39342,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="489"/>
-      <c r="P80" s="503"/>
+      <c r="O80" s="508"/>
+      <c r="P80" s="510"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -39319,8 +39372,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="488"/>
-      <c r="P81" s="502"/>
+      <c r="O81" s="507"/>
+      <c r="P81" s="509"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -39352,8 +39405,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="489"/>
-      <c r="P82" s="503"/>
+      <c r="O82" s="508"/>
+      <c r="P82" s="510"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -39511,8 +39564,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="504"/>
-      <c r="M87" s="505"/>
+      <c r="L87" s="511"/>
+      <c r="M87" s="512"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -39544,8 +39597,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="504"/>
-      <c r="M88" s="505"/>
+      <c r="L88" s="511"/>
+      <c r="M88" s="512"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -39748,8 +39801,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="488"/>
-      <c r="P94" s="498"/>
+      <c r="O94" s="507"/>
+      <c r="P94" s="503"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -39781,8 +39834,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="489"/>
-      <c r="P95" s="499"/>
+      <c r="O95" s="508"/>
+      <c r="P95" s="504"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -45174,11 +45227,11 @@
         <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="500" t="s">
+      <c r="F259" s="505" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="500"/>
-      <c r="H259" s="501"/>
+      <c r="G259" s="505"/>
+      <c r="H259" s="506"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>491400.01</v>
@@ -45752,18 +45805,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O79:O80"/>
+    <mergeCell ref="P79:P80"/>
+    <mergeCell ref="A1:J2"/>
+    <mergeCell ref="S1:T2"/>
     <mergeCell ref="F259:H259"/>
     <mergeCell ref="O81:O82"/>
     <mergeCell ref="P81:P82"/>
     <mergeCell ref="L87:M88"/>
     <mergeCell ref="O94:O95"/>
     <mergeCell ref="P94:P95"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O79:O80"/>
-    <mergeCell ref="P79:P80"/>
-    <mergeCell ref="A1:J2"/>
-    <mergeCell ref="S1:T2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>